<commit_message>
arrumando ainda os kda
</commit_message>
<xml_diff>
--- a/server/dados_1.0.xlsx
+++ b/server/dados_1.0.xlsx
@@ -476,10 +476,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A2" t="n">
+        <v>0</v>
       </c>
       <c r="B2" t="n">
         <v>3000</v>
@@ -492,10 +490,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E2" t="n">
+        <v>0</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -512,10 +508,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A3" t="n">
+        <v>0</v>
       </c>
       <c r="B3" t="n">
         <v>4500</v>
@@ -528,10 +522,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E3" t="n">
+        <v>0</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -548,10 +540,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A4" t="n">
+        <v>0</v>
       </c>
       <c r="B4" t="n">
         <v>6000</v>
@@ -564,10 +554,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E4" t="n">
+        <v>0</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -584,10 +572,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A5" t="n">
+        <v>0</v>
       </c>
       <c r="B5" t="n">
         <v>7500</v>
@@ -600,10 +586,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E5" t="n">
+        <v>0</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -620,10 +604,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A6" t="n">
+        <v>0</v>
       </c>
       <c r="B6" t="n">
         <v>9000</v>
@@ -636,10 +618,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E6" t="n">
+        <v>0</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -656,10 +636,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A7" t="n">
+        <v>0</v>
       </c>
       <c r="B7" t="n">
         <v>10500</v>
@@ -672,10 +650,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E7" t="n">
+        <v>0</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -692,10 +668,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A8" t="n">
+        <v>0</v>
       </c>
       <c r="B8" t="n">
         <v>12000</v>
@@ -708,10 +682,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E8" t="n">
+        <v>0</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -728,10 +700,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A9" t="n">
+        <v>0</v>
       </c>
       <c r="B9" t="n">
         <v>13500</v>
@@ -744,10 +714,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E9" t="n">
+        <v>0</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -764,10 +732,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A10" t="n">
+        <v>0</v>
       </c>
       <c r="B10" t="n">
         <v>15000</v>
@@ -780,10 +746,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E10" t="n">
+        <v>0</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -800,10 +764,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A11" t="n">
+        <v>0</v>
       </c>
       <c r="B11" t="n">
         <v>16500</v>
@@ -816,10 +778,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E11" t="n">
+        <v>0</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -836,10 +796,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A12" t="n">
+        <v>0</v>
       </c>
       <c r="B12" t="n">
         <v>18000</v>
@@ -852,10 +810,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E12" t="n">
+        <v>0</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -872,10 +828,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A13" t="n">
+        <v>1</v>
       </c>
       <c r="B13" t="n">
         <v>19500</v>
@@ -888,10 +842,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E13" t="n">
+        <v>0</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -908,10 +860,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A14" t="n">
+        <v>1</v>
       </c>
       <c r="B14" t="n">
         <v>21000</v>
@@ -924,10 +874,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E14" t="n">
+        <v>0</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -944,10 +892,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A15" t="n">
+        <v>1</v>
       </c>
       <c r="B15" t="n">
         <v>22500</v>
@@ -960,10 +906,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E15" t="n">
+        <v>0</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -980,10 +924,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A16" t="n">
+        <v>1</v>
       </c>
       <c r="B16" t="n">
         <v>24000</v>
@@ -996,10 +938,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E16" t="n">
+        <v>0</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1016,10 +956,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A17" t="n">
+        <v>1</v>
       </c>
       <c r="B17" t="n">
         <v>25500</v>
@@ -1032,10 +970,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E17" t="n">
+        <v>0</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1052,10 +988,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A18" t="n">
+        <v>1</v>
       </c>
       <c r="B18" t="n">
         <v>27000</v>
@@ -1068,10 +1002,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E18" t="n">
+        <v>1</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1088,10 +1020,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A19" t="n">
+        <v>1</v>
       </c>
       <c r="B19" t="n">
         <v>28500</v>
@@ -1104,10 +1034,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E19" t="n">
+        <v>1</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1124,10 +1052,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A20" t="n">
+        <v>1</v>
       </c>
       <c r="B20" t="n">
         <v>30000</v>
@@ -1140,10 +1066,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E20" t="n">
+        <v>1</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1160,10 +1084,8 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A21" t="n">
+        <v>3</v>
       </c>
       <c r="B21" t="n">
         <v>31500</v>
@@ -1176,10 +1098,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E21" t="n">
+        <v>1</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1196,10 +1116,8 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A22" t="n">
+        <v>3</v>
       </c>
       <c r="B22" t="n">
         <v>33000</v>
@@ -1212,10 +1130,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E22" t="n">
+        <v>1</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1232,10 +1148,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A23" t="n">
+        <v>4</v>
       </c>
       <c r="B23" t="n">
         <v>34500</v>
@@ -1248,10 +1162,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="E23" t="n">
+        <v>2</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1268,10 +1180,8 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A24" t="n">
+        <v>4</v>
       </c>
       <c r="B24" t="n">
         <v>36000</v>
@@ -1284,10 +1194,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="E24" t="n">
+        <v>2</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1304,10 +1212,8 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A25" t="n">
+        <v>4</v>
       </c>
       <c r="B25" t="n">
         <v>37500</v>
@@ -1320,10 +1226,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="E25" t="n">
+        <v>3</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1340,10 +1244,8 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A26" t="n">
+        <v>4</v>
       </c>
       <c r="B26" t="n">
         <v>39000</v>
@@ -1356,10 +1258,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="E26" t="n">
+        <v>3</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1376,10 +1276,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A27" t="n">
+        <v>4</v>
       </c>
       <c r="B27" t="n">
         <v>40500</v>
@@ -1392,10 +1290,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="E27" t="n">
+        <v>3</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1412,10 +1308,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A28" t="n">
+        <v>5</v>
       </c>
       <c r="B28" t="n">
         <v>42000</v>
@@ -1428,10 +1322,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="E28" t="n">
+        <v>3</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1448,10 +1340,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A29" t="n">
+        <v>5</v>
       </c>
       <c r="B29" t="n">
         <v>43500</v>
@@ -1464,10 +1354,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="E29" t="n">
+        <v>3</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -1484,10 +1372,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A30" t="n">
+        <v>5</v>
       </c>
       <c r="B30" t="n">
         <v>45000</v>
@@ -1500,10 +1386,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="E30" t="n">
+        <v>3</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1520,10 +1404,8 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A31" t="n">
+        <v>5</v>
       </c>
       <c r="B31" t="n">
         <v>46500</v>
@@ -1536,10 +1418,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="E31" t="n">
+        <v>3</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1556,10 +1436,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A32" t="n">
+        <v>5</v>
       </c>
       <c r="B32" t="n">
         <v>48000</v>
@@ -1572,10 +1450,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="E32" t="n">
+        <v>3</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -1592,10 +1468,8 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A33" t="n">
+        <v>5</v>
       </c>
       <c r="B33" t="n">
         <v>49500</v>
@@ -1608,10 +1482,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="E33" t="n">
+        <v>3</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1628,10 +1500,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A34" t="n">
+        <v>5</v>
       </c>
       <c r="B34" t="n">
         <v>51000</v>
@@ -1644,10 +1514,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="E34" t="n">
+        <v>3</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1664,10 +1532,8 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A35" t="n">
+        <v>5</v>
       </c>
       <c r="B35" t="n">
         <v>52500</v>
@@ -1680,10 +1546,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="E35" t="n">
+        <v>3</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -1700,10 +1564,8 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A36" t="n">
+        <v>5</v>
       </c>
       <c r="B36" t="n">
         <v>54000</v>
@@ -1716,10 +1578,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="E36" t="n">
+        <v>3</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -1736,10 +1596,8 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A37" t="n">
+        <v>5</v>
       </c>
       <c r="B37" t="n">
         <v>55500</v>
@@ -1752,10 +1610,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="E37" t="n">
+        <v>4</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1772,10 +1628,8 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A38" t="n">
+        <v>5</v>
       </c>
       <c r="B38" t="n">
         <v>57000</v>
@@ -1788,10 +1642,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="E38" t="n">
+        <v>4</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -1808,10 +1660,8 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A39" t="n">
+        <v>5</v>
       </c>
       <c r="B39" t="n">
         <v>58500</v>
@@ -1824,10 +1674,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="E39" t="n">
+        <v>4</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -1844,10 +1692,8 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A40" t="n">
+        <v>5</v>
       </c>
       <c r="B40" t="n">
         <v>60000</v>
@@ -1860,10 +1706,8 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="E40" t="n">
+        <v>4</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -1880,10 +1724,8 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>erro</t>
-        </is>
+      <c r="A41" t="n">
+        <v>5</v>
       </c>
       <c r="B41" t="n">
         <v>61500</v>
@@ -1896,14 +1738,12 @@
           <t>BLUE</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>erro</t>
-        </is>
+      <c r="E41" t="n">
+        <v>4</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>erro</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G41" t="n">

</xml_diff>

<commit_message>
arrumando os champs certo
</commit_message>
<xml_diff>
--- a/server/dados_1.0.xlsx
+++ b/server/dados_1.0.xlsx
@@ -493,10 +493,8 @@
       <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="F2" t="n">
+        <v>0</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -525,10 +523,8 @@
       <c r="E3" t="n">
         <v>0</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="F3" t="n">
+        <v>0</v>
       </c>
       <c r="G3" t="n">
         <v>8</v>
@@ -557,10 +553,8 @@
       <c r="E4" t="n">
         <v>0</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="F4" t="n">
+        <v>0</v>
       </c>
       <c r="G4" t="n">
         <v>17</v>
@@ -589,17 +583,15 @@
       <c r="E5" t="n">
         <v>0</v>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="F5" t="n">
+        <v>0</v>
       </c>
       <c r="G5" t="n">
         <v>24</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Ornn</t>
+          <t>Yone</t>
         </is>
       </c>
     </row>
@@ -621,10 +613,8 @@
       <c r="E6" t="n">
         <v>0</v>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="F6" t="n">
+        <v>0</v>
       </c>
       <c r="G6" t="n">
         <v>33</v>
@@ -653,10 +643,8 @@
       <c r="E7" t="n">
         <v>0</v>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="F7" t="n">
+        <v>0</v>
       </c>
       <c r="G7" t="n">
         <v>38</v>
@@ -685,10 +673,8 @@
       <c r="E8" t="n">
         <v>0</v>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="F8" t="n">
+        <v>0</v>
       </c>
       <c r="G8" t="n">
         <v>52</v>
@@ -717,10 +703,8 @@
       <c r="E9" t="n">
         <v>0</v>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="F9" t="n">
+        <v>0</v>
       </c>
       <c r="G9" t="n">
         <v>65</v>
@@ -749,10 +733,8 @@
       <c r="E10" t="n">
         <v>0</v>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="F10" t="n">
+        <v>0</v>
       </c>
       <c r="G10" t="n">
         <v>76</v>
@@ -781,17 +763,15 @@
       <c r="E11" t="n">
         <v>0</v>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="F11" t="n">
+        <v>0</v>
       </c>
       <c r="G11" t="n">
         <v>83</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Pyke</t>
+          <t>Yone</t>
         </is>
       </c>
     </row>
@@ -813,10 +793,8 @@
       <c r="E12" t="n">
         <v>0</v>
       </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="F12" t="n">
+        <v>0</v>
       </c>
       <c r="G12" t="n">
         <v>88</v>
@@ -845,10 +823,8 @@
       <c r="E13" t="n">
         <v>0</v>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="F13" t="n">
+        <v>0</v>
       </c>
       <c r="G13" t="n">
         <v>104</v>
@@ -877,10 +853,8 @@
       <c r="E14" t="n">
         <v>0</v>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="F14" t="n">
+        <v>0</v>
       </c>
       <c r="G14" t="n">
         <v>110</v>
@@ -909,10 +883,8 @@
       <c r="E15" t="n">
         <v>0</v>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="F15" t="n">
+        <v>0</v>
       </c>
       <c r="G15" t="n">
         <v>116</v>
@@ -941,10 +913,8 @@
       <c r="E16" t="n">
         <v>0</v>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="F16" t="n">
+        <v>0</v>
       </c>
       <c r="G16" t="n">
         <v>130</v>
@@ -973,17 +943,15 @@
       <c r="E17" t="n">
         <v>0</v>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="F17" t="n">
+        <v>0</v>
       </c>
       <c r="G17" t="n">
         <v>139</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Pyke</t>
+          <t>Yone</t>
         </is>
       </c>
     </row>
@@ -1005,10 +973,8 @@
       <c r="E18" t="n">
         <v>1</v>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="F18" t="n">
+        <v>0</v>
       </c>
       <c r="G18" t="n">
         <v>142</v>
@@ -1037,10 +1003,8 @@
       <c r="E19" t="n">
         <v>1</v>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="F19" t="n">
+        <v>0</v>
       </c>
       <c r="G19" t="n">
         <v>156</v>
@@ -1069,10 +1033,8 @@
       <c r="E20" t="n">
         <v>1</v>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="F20" t="n">
+        <v>0</v>
       </c>
       <c r="G20" t="n">
         <v>160</v>
@@ -1101,10 +1063,8 @@
       <c r="E21" t="n">
         <v>1</v>
       </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="F21" t="n">
+        <v>2</v>
       </c>
       <c r="G21" t="n">
         <v>163</v>
@@ -1133,10 +1093,8 @@
       <c r="E22" t="n">
         <v>1</v>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="F22" t="n">
+        <v>2</v>
       </c>
       <c r="G22" t="n">
         <v>174</v>
@@ -1165,17 +1123,15 @@
       <c r="E23" t="n">
         <v>2</v>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="F23" t="n">
+        <v>2</v>
       </c>
       <c r="G23" t="n">
         <v>182</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Pyke</t>
+          <t>Yone</t>
         </is>
       </c>
     </row>
@@ -1197,10 +1153,8 @@
       <c r="E24" t="n">
         <v>2</v>
       </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="F24" t="n">
+        <v>2</v>
       </c>
       <c r="G24" t="n">
         <v>189</v>
@@ -1229,17 +1183,15 @@
       <c r="E25" t="n">
         <v>3</v>
       </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="F25" t="n">
+        <v>2</v>
       </c>
       <c r="G25" t="n">
         <v>189</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Ksante</t>
+          <t>Yone</t>
         </is>
       </c>
     </row>
@@ -1261,10 +1213,8 @@
       <c r="E26" t="n">
         <v>3</v>
       </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="F26" t="n">
+        <v>2</v>
       </c>
       <c r="G26" t="n">
         <v>195</v>
@@ -1293,10 +1243,8 @@
       <c r="E27" t="n">
         <v>3</v>
       </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="F27" t="n">
+        <v>2</v>
       </c>
       <c r="G27" t="n">
         <v>205</v>
@@ -1325,10 +1273,8 @@
       <c r="E28" t="n">
         <v>3</v>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="F28" t="n">
+        <v>2</v>
       </c>
       <c r="G28" t="n">
         <v>214</v>
@@ -1357,17 +1303,15 @@
       <c r="E29" t="n">
         <v>3</v>
       </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="F29" t="n">
+        <v>2</v>
       </c>
       <c r="G29" t="n">
         <v>222</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Pyke</t>
+          <t>Yone</t>
         </is>
       </c>
     </row>
@@ -1389,10 +1333,8 @@
       <c r="E30" t="n">
         <v>3</v>
       </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="F30" t="n">
+        <v>2</v>
       </c>
       <c r="G30" t="n">
         <v>242</v>
@@ -1421,10 +1363,8 @@
       <c r="E31" t="n">
         <v>3</v>
       </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="F31" t="n">
+        <v>2</v>
       </c>
       <c r="G31" t="n">
         <v>248</v>
@@ -1453,10 +1393,8 @@
       <c r="E32" t="n">
         <v>3</v>
       </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="F32" t="n">
+        <v>2</v>
       </c>
       <c r="G32" t="n">
         <v>251</v>
@@ -1485,10 +1423,8 @@
       <c r="E33" t="n">
         <v>3</v>
       </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="F33" t="n">
+        <v>2</v>
       </c>
       <c r="G33" t="n">
         <v>261</v>
@@ -1517,10 +1453,8 @@
       <c r="E34" t="n">
         <v>3</v>
       </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="F34" t="n">
+        <v>2</v>
       </c>
       <c r="G34" t="n">
         <v>274</v>
@@ -1549,17 +1483,15 @@
       <c r="E35" t="n">
         <v>3</v>
       </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="F35" t="n">
+        <v>2</v>
       </c>
       <c r="G35" t="n">
         <v>281</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Pyke</t>
+          <t>Yone</t>
         </is>
       </c>
     </row>
@@ -1581,10 +1513,8 @@
       <c r="E36" t="n">
         <v>3</v>
       </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="F36" t="n">
+        <v>3</v>
       </c>
       <c r="G36" t="n">
         <v>281</v>
@@ -1613,17 +1543,15 @@
       <c r="E37" t="n">
         <v>4</v>
       </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="F37" t="n">
+        <v>3</v>
       </c>
       <c r="G37" t="n">
         <v>28</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Taliyah</t>
+          <t>Yone</t>
         </is>
       </c>
     </row>
@@ -1645,10 +1573,8 @@
       <c r="E38" t="n">
         <v>4</v>
       </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="F38" t="n">
+        <v>3</v>
       </c>
       <c r="G38" t="n">
         <v>284</v>
@@ -1677,10 +1603,8 @@
       <c r="E39" t="n">
         <v>4</v>
       </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="F39" t="n">
+        <v>3</v>
       </c>
       <c r="G39" t="n">
         <v>294</v>
@@ -1709,10 +1633,8 @@
       <c r="E40" t="n">
         <v>4</v>
       </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="F40" t="n">
+        <v>3</v>
       </c>
       <c r="G40" t="n">
         <v>299</v>
@@ -1741,17 +1663,15 @@
       <c r="E41" t="n">
         <v>4</v>
       </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="F41" t="n">
+        <v>3</v>
       </c>
       <c r="G41" t="n">
         <v>0</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Ornn</t>
+          <t>Yone</t>
         </is>
       </c>
     </row>

</xml_diff>